<commit_message>
improved graph for use in lab log
</commit_message>
<xml_diff>
--- a/weighted_averaging_graph.xlsx
+++ b/weighted_averaging_graph.xlsx
@@ -114,6 +114,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Plot</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>  demonstrating weighted average calculation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -155,15 +185,23 @@
           <c:order val="0"/>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="x"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -235,6 +273,206 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D547-48F4-8C2C-402B6BDEE93F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>series 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$I$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-127</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>127</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$I$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>253</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D547-48F4-8C2C-402B6BDEE93F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Series 3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$I$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-127</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>127</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>251</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D547-48F4-8C2C-402B6BDEE93F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -272,6 +510,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Line position (abritrary</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> units)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="in"/>
@@ -319,6 +618,8 @@
         <c:axId val="353057544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="256"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -336,6 +637,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Reflectivity (out</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> of 255)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -376,6 +738,7 @@
         <c:crossAx val="353056888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="32"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -983,15 +1346,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>181428</xdr:colOff>
+      <xdr:colOff>90714</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>272143</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>174171</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1013,15 +1376,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>145142</xdr:rowOff>
+      <xdr:colOff>226786</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>45357</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
+      <xdr:colOff>226786</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>145143</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1030,12 +1393,113 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5306786" y="1596571"/>
-          <a:ext cx="0" cy="2358572"/>
+          <a:off x="5089072" y="1859643"/>
+          <a:ext cx="0" cy="2013857"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln w="15875"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>544285</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>45357</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>544285</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Connector 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3583214" y="1859643"/>
+          <a:ext cx="0" cy="2013857"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>36285</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Connector 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1850571" y="1850571"/>
+          <a:ext cx="0" cy="2013857"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -1323,7 +1787,7 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>